<commit_message>
Modify the path of runcommand.bat and write file path.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/600.20.20.100_UserCanNotConfigureActionSetWithoutConfigureActionPermission.xlsx
+++ b/NformTester/NformTester/Keywordscripts/600.20.20.100_UserCanNotConfigureActionSetWithoutConfigureActionPermission.xlsx
@@ -3649,9 +3649,6 @@
     <t>"Write file testing"</t>
   </si>
   <si>
-    <t>"C:\Nform\test.txt"</t>
-  </si>
-  <si>
     <t>"test"</t>
   </si>
   <si>
@@ -3703,6 +3700,10 @@
   </si>
   <si>
     <t>;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"C:\test.txt"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4662,8 +4663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="E37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4795,7 +4796,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>197</v>
@@ -5162,7 +5163,7 @@
         <v>4</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>804</v>
+        <v>821</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -5193,7 +5194,7 @@
         <v>4</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -5328,7 +5329,7 @@
         <v>21</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -5440,7 +5441,7 @@
         <v>4</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
@@ -5466,7 +5467,7 @@
         <v>4</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
@@ -5516,10 +5517,10 @@
         <v>7</v>
       </c>
       <c r="H29" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="I29" s="5" t="s">
         <v>809</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>810</v>
       </c>
       <c r="J29" s="5" t="b">
         <v>0</v>
@@ -5546,10 +5547,10 @@
         <v>7</v>
       </c>
       <c r="H30" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="I30" s="5" t="s">
         <v>809</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>810</v>
       </c>
       <c r="J30" s="5" t="b">
         <v>0</v>
@@ -5576,10 +5577,10 @@
         <v>7</v>
       </c>
       <c r="H31" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="I31" s="5" t="s">
         <v>809</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>810</v>
       </c>
       <c r="J31" s="5" t="b">
         <v>0</v>
@@ -5606,10 +5607,10 @@
         <v>7</v>
       </c>
       <c r="H32" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="I32" s="5" t="s">
         <v>809</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>810</v>
       </c>
       <c r="J32" s="5" t="b">
         <v>0</v>
@@ -5636,10 +5637,10 @@
         <v>7</v>
       </c>
       <c r="H33" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="I33" s="5" t="s">
         <v>809</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>810</v>
       </c>
       <c r="J33" s="5" t="b">
         <v>0</v>
@@ -5666,10 +5667,10 @@
         <v>7</v>
       </c>
       <c r="H34" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="I34" s="5" t="s">
         <v>809</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>810</v>
       </c>
       <c r="J34" s="5" t="b">
         <v>0</v>
@@ -5732,7 +5733,7 @@
         <v>36</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -5762,7 +5763,7 @@
         <v>4</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
@@ -5788,7 +5789,7 @@
         <v>4</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
@@ -5814,7 +5815,7 @@
         <v>4</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
@@ -5840,7 +5841,7 @@
         <v>4</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
@@ -5866,7 +5867,7 @@
         <v>13</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
@@ -5952,7 +5953,7 @@
         <v>45</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -6028,7 +6029,7 @@
       </c>
       <c r="G49" s="5"/>
       <c r="H49" s="11" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>796</v>
@@ -6132,10 +6133,10 @@
         <v>7</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="J53" s="5" t="b">
         <v>0</v>
@@ -6162,10 +6163,10 @@
         <v>7</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="J54" s="5" t="b">
         <v>0</v>
@@ -6192,13 +6193,13 @@
         <v>7</v>
       </c>
       <c r="H55" s="5" t="s">
+        <v>816</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="J55" s="5" t="s">
         <v>817</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>810</v>
-      </c>
-      <c r="J55" s="5" t="s">
-        <v>818</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
@@ -6222,10 +6223,10 @@
         <v>7</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="J56" s="5" t="s">
         <v>184</v>
@@ -6264,7 +6265,7 @@
         <v>57</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
@@ -6354,7 +6355,7 @@
         <v>61</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>197</v>
@@ -6552,7 +6553,7 @@
         <v>56</v>
       </c>
       <c r="H70" s="11" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="I70" s="5"/>
       <c r="J70" s="5"/>
@@ -6600,7 +6601,7 @@
         <v>56</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>

</xml_diff>